<commit_message>
Analysis for excel sheet
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,24 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julisa\Documents\RFBF\RFBF.repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E888EA4-6E4A-4EC8-AE3B-3CEF19CB6B88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D7CD59-F2DB-4109-B1A6-14671E9D006F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="5" xr2:uid="{0CC1065D-DCA8-C146-8D90-857D37AD70DB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" firstSheet="6" activeTab="9" xr2:uid="{0CC1065D-DCA8-C146-8D90-857D37AD70DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Study Info" sheetId="2" r:id="rId1"/>
     <sheet name="Acceptability" sheetId="1" r:id="rId2"/>
-    <sheet name="RM Paths" sheetId="3" r:id="rId3"/>
-    <sheet name="IN Paths" sheetId="4" r:id="rId4"/>
-    <sheet name="All Paths" sheetId="5" r:id="rId5"/>
-    <sheet name="RM Item Analysis" sheetId="6" r:id="rId6"/>
-    <sheet name="Order Effects" sheetId="7" r:id="rId7"/>
-    <sheet name="Main Effects" sheetId="10" r:id="rId8"/>
-    <sheet name="Simple Slopes" sheetId="9" r:id="rId9"/>
-    <sheet name="Mean Differences" sheetId="8" r:id="rId10"/>
+    <sheet name="Midpoint" sheetId="12" r:id="rId3"/>
+    <sheet name="RM Paths" sheetId="3" r:id="rId4"/>
+    <sheet name="IN Paths" sheetId="4" r:id="rId5"/>
+    <sheet name="All Paths" sheetId="5" r:id="rId6"/>
+    <sheet name="RM Item Analysis" sheetId="6" r:id="rId7"/>
+    <sheet name="RM Factor Analysis" sheetId="13" r:id="rId8"/>
+    <sheet name="Order Effects" sheetId="7" r:id="rId9"/>
+    <sheet name="Main Effects" sheetId="10" r:id="rId10"/>
+    <sheet name="Simple Slopes" sheetId="9" r:id="rId11"/>
+    <sheet name="Mean Differences" sheetId="8" r:id="rId12"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId11"/>
+    <externalReference r:id="rId13"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="111">
   <si>
     <t>df</t>
   </si>
@@ -101,12 +103,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>In paper?</t>
-  </si>
-  <si>
-    <t>Preregistered?</t>
-  </si>
-  <si>
     <t>College</t>
   </si>
   <si>
@@ -284,26 +280,113 @@
     <t xml:space="preserve">Study 1A </t>
   </si>
   <si>
-    <t>BF first Mean</t>
-  </si>
-  <si>
-    <t>RF first Mean</t>
-  </si>
-  <si>
     <t>Race</t>
   </si>
   <si>
-    <t>Mix</t>
-  </si>
-  <si>
-    <t>White</t>
+    <t>Denial of Disparities</t>
+  </si>
+  <si>
+    <t>Unawareness of Racial Privelege</t>
+  </si>
+  <si>
+    <t>Random Order</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>57% Asian, 21% White, 11% Other, 11% NA</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>% of FGC</t>
+  </si>
+  <si>
+    <t>Midpoint</t>
+  </si>
+  <si>
+    <t>41% women, 58% men</t>
+  </si>
+  <si>
+    <t>57% women, 41% men</t>
+  </si>
+  <si>
+    <t>54% Asian, 23% White, 14% Other, 7% NA</t>
+  </si>
+  <si>
+    <t>Mono-Racial White</t>
+  </si>
+  <si>
+    <t>RacismMini_1.1</t>
+  </si>
+  <si>
+    <t>RacismMini_2.1</t>
+  </si>
+  <si>
+    <t>RacismMini_3.1</t>
+  </si>
+  <si>
+    <t>RacismMini_4.1</t>
+  </si>
+  <si>
+    <t>RacismMini_5.1</t>
+  </si>
+  <si>
+    <t>RacismMini_6.1</t>
+  </si>
+  <si>
+    <t>RacismMini_7.1</t>
+  </si>
+  <si>
+    <t>RacismMini_8.1</t>
+  </si>
+  <si>
+    <t>RacismMini_9.1</t>
+  </si>
+  <si>
+    <t>RacismMini_10.1</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Factor 1</t>
+  </si>
+  <si>
+    <t>Factor 2</t>
+  </si>
+  <si>
+    <t>Blk Race Mini</t>
+  </si>
+  <si>
+    <t>Ntv Race Mini</t>
+  </si>
+  <si>
+    <t>Overall Race Mini</t>
+  </si>
+  <si>
+    <t>44% women, 55% men</t>
+  </si>
+  <si>
+    <t>49% women, 50% men</t>
+  </si>
+  <si>
+    <t>52% women, 47% men</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -327,6 +410,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -406,7 +496,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -486,12 +576,394 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -538,82 +1010,383 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -624,8 +1397,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFEDDBFF"/>
       <color rgb="FFDEBDFF"/>
-      <color rgb="FFEDDBFF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -725,7 +1498,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'RM Item Analysis'!$B$1</c:f>
+              <c:f>'RM Item Analysis'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -746,7 +1519,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'RM Item Analysis'!$A$2:$A$11</c:f>
+              <c:f>'RM Item Analysis'!$B$2:$B$11</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -784,7 +1557,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'RM Item Analysis'!$B$2:$B$11</c:f>
+              <c:f>'RM Item Analysis'!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -832,7 +1605,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'RM Item Analysis'!$C$1</c:f>
+              <c:f>'RM Item Analysis'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -853,7 +1626,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'RM Item Analysis'!$A$2:$A$11</c:f>
+              <c:f>'RM Item Analysis'!$B$2:$B$11</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -891,7 +1664,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'RM Item Analysis'!$C$2:$C$11</c:f>
+              <c:f>'RM Item Analysis'!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1223,7 +1996,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'RM Item Analysis'!$B$38</c:f>
+              <c:f>'RM Item Analysis'!$C$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1244,7 +2017,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'RM Item Analysis'!$A$39:$A$48</c:f>
+              <c:f>'RM Item Analysis'!$B$39:$B$48</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1282,7 +2055,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'RM Item Analysis'!$B$39:$B$48</c:f>
+              <c:f>'RM Item Analysis'!$C$39:$C$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1330,7 +2103,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'RM Item Analysis'!$C$38</c:f>
+              <c:f>'RM Item Analysis'!$D$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1351,7 +2124,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'RM Item Analysis'!$A$39:$A$48</c:f>
+              <c:f>'RM Item Analysis'!$B$39:$B$48</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1389,7 +2162,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'RM Item Analysis'!$C$39:$C$48</c:f>
+              <c:f>'RM Item Analysis'!$D$39:$D$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1721,7 +2494,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'RM Item Analysis'!$B$51</c:f>
+              <c:f>'RM Item Analysis'!$C$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1742,7 +2515,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'RM Item Analysis'!$A$52:$A$61</c:f>
+              <c:f>'RM Item Analysis'!$B$52:$B$61</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1780,7 +2553,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'RM Item Analysis'!$B$52:$B$61</c:f>
+              <c:f>'RM Item Analysis'!$C$52:$C$61</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1828,7 +2601,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'RM Item Analysis'!$C$51</c:f>
+              <c:f>'RM Item Analysis'!$D$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1849,7 +2622,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'RM Item Analysis'!$A$52:$A$61</c:f>
+              <c:f>'RM Item Analysis'!$B$52:$B$61</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1887,7 +2660,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'RM Item Analysis'!$C$52:$C$61</c:f>
+              <c:f>'RM Item Analysis'!$D$52:$D$61</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3766,13 +4539,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>178592</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>140493</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>4763</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
@@ -3804,13 +4577,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>169066</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>135730</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>623887</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>52388</xdr:rowOff>
@@ -3842,13 +4615,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>190716</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>145688</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>443779</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>64943</xdr:rowOff>
@@ -4546,155 +5319,196 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A14ED6-79EE-421B-9E46-BFF6F0414071}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="2" width="10.9375" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="1" max="1" width="20.5" style="50" customWidth="1"/>
+    <col min="2" max="2" width="10.9375" style="50" customWidth="1"/>
+    <col min="3" max="3" width="7.3125" style="50" customWidth="1"/>
+    <col min="4" max="4" width="9" style="50"/>
+    <col min="5" max="5" width="7.5" style="50" customWidth="1"/>
+    <col min="6" max="6" width="21.125" style="50" customWidth="1"/>
+    <col min="7" max="7" width="14.8125" style="50" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A1" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" s="20" t="s">
+      <c r="D1" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" s="52" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A2" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="C2" s="50">
+        <v>75</v>
+      </c>
+      <c r="D2" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="20" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A2" s="9" t="s">
+      <c r="E2" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="53">
+        <v>0.31</v>
+      </c>
+      <c r="I2" s="50">
+        <v>19.07</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A3" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="50">
+        <v>102</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="53">
+        <v>0.26</v>
+      </c>
+      <c r="I3" s="50">
+        <v>19.02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A4" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B4" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="50">
+        <v>148</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="G4" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="H4" s="53">
+        <v>0.15</v>
+      </c>
+      <c r="I4" s="50">
+        <v>19.09</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A5" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="50">
+        <v>648</v>
+      </c>
+      <c r="D5" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="9">
-        <v>86</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="9" t="s">
+      <c r="F5" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="G5" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="H5" s="53">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I5" s="50">
+        <v>38.07</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A6" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="50">
+        <v>774</v>
+      </c>
+      <c r="D6" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="9">
-        <v>108</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="9">
-        <v>150</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A5" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="9">
-        <v>733</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A6" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="9">
-        <v>900</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>83</v>
+      <c r="F6" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" s="50" t="s">
+        <v>110</v>
+      </c>
+      <c r="H6" s="53">
+        <v>0.49</v>
+      </c>
+      <c r="I6" s="50">
+        <v>38.700000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -4703,6 +5517,32 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB1568F0-3754-4110-ADDE-1A6EDD471F19}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A4FC0C-94F6-4EE7-A7D0-F02B7768E222}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04D04D31-CEA1-4D70-8FC8-63966FE1EC8A}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -4720,8 +5560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D48CA9C-3CF7-AA49-BF49-968890DCA86C}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" zoomScale="187" zoomScaleNormal="187" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -4731,7 +5571,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A1" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -4748,24 +5588,24 @@
       <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="22" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A2" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="A2" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A3" s="4" t="s">
@@ -4775,16 +5615,16 @@
         <v>3.02</v>
       </c>
       <c r="C3" s="6">
-        <v>3.34</v>
+        <v>3.32</v>
       </c>
       <c r="D3" s="6">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E3" s="6">
-        <v>-3.097</v>
+        <v>-2.9</v>
       </c>
       <c r="F3" s="6">
-        <v>3.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.5">
@@ -4792,10 +5632,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="6">
-        <v>1.1299999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="C4" s="6">
-        <v>1.1200000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -4806,7 +5646,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="6">
-        <v>0.92200000000000004</v>
+        <v>0.92300000000000004</v>
       </c>
       <c r="C5" s="6">
         <v>0.93500000000000005</v>
@@ -4816,43 +5656,43 @@
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="8">
         <v>2.8</v>
       </c>
       <c r="C7" s="8">
-        <v>3.1419999999999999</v>
+        <v>3.14</v>
       </c>
       <c r="D7" s="8">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E7" s="8">
-        <v>-3.4780000000000002</v>
+        <v>-3.38</v>
       </c>
       <c r="F7" s="8">
-        <v>6.9999999999999999E-4</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="8">
-        <v>1.32</v>
+        <v>1.33</v>
       </c>
       <c r="C8" s="8">
         <v>1.28</v>
@@ -4862,11 +5702,11 @@
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="20" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="8">
-        <v>0.92200000000000004</v>
+        <v>0.92400000000000004</v>
       </c>
       <c r="C9" s="8">
         <v>0.71</v>
@@ -4876,35 +5716,35 @@
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="27"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="43"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="21" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="8">
-        <v>2.41</v>
+        <v>2.33</v>
       </c>
       <c r="C11" s="8">
-        <v>2.83</v>
+        <v>2.84</v>
       </c>
       <c r="D11" s="8">
-        <v>174</v>
+        <v>146</v>
       </c>
       <c r="E11" s="8">
-        <v>2.2400000000000002</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="F11" s="8">
-        <v>2.5999999999999999E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="G11" s="8">
         <v>0.28299999999999997</v>
@@ -4914,14 +5754,14 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="8">
-        <v>1.32</v>
+        <v>1.31</v>
       </c>
       <c r="C12" s="8">
-        <v>1.1499999999999999</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -4930,14 +5770,14 @@
       <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="21" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="8">
-        <v>0.95699999999999996</v>
+        <v>0.95599999999999996</v>
       </c>
       <c r="C13" s="8">
-        <v>0.92500000000000004</v>
+        <v>0.95099999999999996</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
@@ -4946,29 +5786,29 @@
       <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="31"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="46"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="8">
-        <v>2.69</v>
+        <v>2.66</v>
       </c>
       <c r="C15" s="8">
-        <v>3.51</v>
+        <v>3.52</v>
       </c>
       <c r="D15" s="8">
-        <v>716</v>
+        <v>644</v>
       </c>
       <c r="E15" s="8">
         <v>8.48</v>
@@ -4988,10 +5828,10 @@
         <v>6</v>
       </c>
       <c r="B16" s="8">
-        <v>1.27</v>
+        <v>1.29</v>
       </c>
       <c r="C16" s="8">
-        <v>1.28</v>
+        <v>1.29</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -5004,10 +5844,10 @@
         <v>7</v>
       </c>
       <c r="B17" s="8">
-        <v>0.95</v>
+        <v>0.95699999999999996</v>
       </c>
       <c r="C17" s="8">
-        <v>0.95</v>
+        <v>0.95099999999999996</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
@@ -5016,32 +5856,32 @@
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="23"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="49"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A19" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="8">
-        <v>2.83</v>
+        <v>2.85</v>
       </c>
       <c r="C19" s="8">
-        <v>3.42</v>
+        <v>3.44</v>
       </c>
       <c r="D19" s="8">
-        <v>911</v>
+        <v>772</v>
       </c>
       <c r="E19" s="8">
-        <v>20.21</v>
+        <v>18.11</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>14</v>
@@ -5054,7 +5894,7 @@
         <v>6</v>
       </c>
       <c r="B20" s="8">
-        <v>1.26</v>
+        <v>1.27</v>
       </c>
       <c r="C20" s="8">
         <v>1.39</v>
@@ -5070,10 +5910,10 @@
         <v>7</v>
       </c>
       <c r="B21" s="8">
-        <v>0.91</v>
+        <v>0.91400000000000003</v>
       </c>
       <c r="C21" s="8">
-        <v>0.92</v>
+        <v>0.92800000000000005</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -5094,10 +5934,200 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{419FBFCB-9157-45B6-9066-DB4DE1EE8502}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A1" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="73" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="74" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="75" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A2" s="79" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="64">
+        <v>3.02</v>
+      </c>
+      <c r="C2" s="60">
+        <v>4</v>
+      </c>
+      <c r="D2" s="60">
+        <v>-7.38</v>
+      </c>
+      <c r="E2" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="64">
+        <v>3.32</v>
+      </c>
+      <c r="G2" s="60">
+        <v>4</v>
+      </c>
+      <c r="H2" s="60">
+        <v>-5.37</v>
+      </c>
+      <c r="I2" s="67" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A3" s="80" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="65">
+        <v>2.8</v>
+      </c>
+      <c r="C3" s="61">
+        <v>4</v>
+      </c>
+      <c r="D3" s="61">
+        <v>-9.11</v>
+      </c>
+      <c r="E3" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="65">
+        <v>3.1419999999999999</v>
+      </c>
+      <c r="G3" s="61">
+        <v>4</v>
+      </c>
+      <c r="H3" s="61">
+        <v>-6.76</v>
+      </c>
+      <c r="I3" s="76" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A4" s="81" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="66">
+        <v>2.41</v>
+      </c>
+      <c r="C4" s="62">
+        <v>4</v>
+      </c>
+      <c r="D4" s="62">
+        <v>-10.92</v>
+      </c>
+      <c r="E4" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="66">
+        <v>2.83</v>
+      </c>
+      <c r="G4" s="62">
+        <v>4</v>
+      </c>
+      <c r="H4" s="62">
+        <v>-8.92</v>
+      </c>
+      <c r="I4" s="68" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A5" s="82" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="65">
+        <v>2.69</v>
+      </c>
+      <c r="C5" s="61">
+        <v>4</v>
+      </c>
+      <c r="D5" s="61">
+        <v>-18.66</v>
+      </c>
+      <c r="E5" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="65">
+        <v>3.51</v>
+      </c>
+      <c r="G5" s="61">
+        <v>4</v>
+      </c>
+      <c r="H5" s="61">
+        <v>-6.73</v>
+      </c>
+      <c r="I5" s="76" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="83" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="69">
+        <v>2.83</v>
+      </c>
+      <c r="C6" s="70">
+        <v>4</v>
+      </c>
+      <c r="D6" s="70">
+        <v>-25.21</v>
+      </c>
+      <c r="E6" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="72">
+        <v>3.42</v>
+      </c>
+      <c r="G6" s="70">
+        <v>4</v>
+      </c>
+      <c r="H6" s="70">
+        <v>-11.17</v>
+      </c>
+      <c r="I6" s="77" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4096C72D-F257-4750-85E8-D54732B0680F}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
+    <sheetView zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
@@ -5126,13 +6156,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A2" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>2</v>
@@ -5141,7 +6171,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>2</v>
@@ -5150,7 +6180,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>2</v>
@@ -5158,7 +6188,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A3" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="9">
         <v>0.29099999999999998</v>
@@ -5190,7 +6220,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A4" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" s="9">
         <v>0.53100000000000003</v>
@@ -5222,7 +6252,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A5" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="9">
         <v>0.28399999999999997</v>
@@ -5254,7 +6284,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A6" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" s="9">
         <v>0.155</v>
@@ -5279,7 +6309,7 @@
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -5292,7 +6322,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F49EA0-0ABB-4877-8E0E-C8126C63F49B}">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -5320,13 +6350,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>2</v>
@@ -5335,7 +6365,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G2" s="16" t="s">
         <v>2</v>
@@ -5343,7 +6373,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" s="9">
         <v>1.37</v>
@@ -5366,7 +6396,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" s="9">
         <v>0.14599999999999999</v>
@@ -5389,7 +6419,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="9">
         <v>0.60799999999999998</v>
@@ -5412,7 +6442,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6" s="9">
         <v>0.2</v>
@@ -5428,7 +6458,7 @@
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -5440,7 +6470,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BE041D1-E0BD-4AA0-8DAA-61EA9689E5FE}">
   <dimension ref="A1:J9"/>
   <sheetViews>
@@ -5473,13 +6503,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A2" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>2</v>
@@ -5488,7 +6518,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>2</v>
@@ -5497,7 +6527,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>2</v>
@@ -5505,7 +6535,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A3" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E3" s="9">
         <v>1.37</v>
@@ -5528,7 +6558,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A4" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" s="9">
         <v>0.29099999999999998</v>
@@ -5560,7 +6590,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A5" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E5" s="9">
         <v>0.14599999999999999</v>
@@ -5583,7 +6613,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A6" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B6" s="9">
         <v>0.53100000000000003</v>
@@ -5615,7 +6645,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A7" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B7" s="9">
         <v>0.28399999999999997</v>
@@ -5647,7 +6677,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A8" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E8" s="9">
         <v>0.2</v>
@@ -5663,12 +6693,12 @@
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A9" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="9">
         <v>0.155</v>
@@ -5693,7 +6723,7 @@
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -5706,12 +6736,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{417F5AD6-A761-4F1C-9919-3044C5F18346}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="O43" sqref="O43"/>
+    <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5719,402 +6749,1170 @@
     <col min="1" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B1" s="19" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="C1" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C2" s="19">
+        <v>3.4420000000000002</v>
+      </c>
+      <c r="D2" s="19">
+        <v>3.5059999999999998</v>
+      </c>
+      <c r="F2" s="19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="19" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="28"/>
+      <c r="B3" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="19">
-        <v>3.4420000000000002</v>
-      </c>
-      <c r="C2" s="19">
-        <v>3.5059999999999998</v>
-      </c>
-      <c r="E2" s="19" t="s">
+      <c r="C3" s="19">
+        <v>3.2090000000000001</v>
+      </c>
+      <c r="D3" s="19">
+        <v>2.9660000000000002</v>
+      </c>
+      <c r="F3" s="19" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="19" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="28"/>
+      <c r="B4" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="19">
-        <v>3.2090000000000001</v>
-      </c>
-      <c r="C3" s="19">
+      <c r="C4" s="19">
+        <v>3.1280000000000001</v>
+      </c>
+      <c r="D4" s="19">
+        <v>3.2469999999999999</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="28"/>
+      <c r="B5" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="19">
         <v>2.9660000000000002</v>
       </c>
-      <c r="E3" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="19" t="s">
+      <c r="D5" s="19">
+        <v>2.8540000000000001</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="28"/>
+      <c r="B6" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="19">
+        <v>2.6859999999999999</v>
+      </c>
+      <c r="D6" s="19">
+        <v>2.7530000000000001</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="28"/>
+      <c r="B7" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="19">
+        <v>2.57</v>
+      </c>
+      <c r="D7" s="19">
+        <v>2.6070000000000002</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="28"/>
+      <c r="B8" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="19">
+        <v>2.1509999999999998</v>
+      </c>
+      <c r="D8" s="19">
+        <v>3.4039999999999999</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="19">
+        <v>2.093</v>
+      </c>
+      <c r="D9" s="19">
+        <v>2.5390000000000001</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="28"/>
+      <c r="B10" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="19">
+        <v>2.2330000000000001</v>
+      </c>
+      <c r="D10" s="19">
+        <v>2.7730000000000001</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="28"/>
+      <c r="B11" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="19">
+        <v>2.419</v>
+      </c>
+      <c r="D11" s="19">
+        <v>3.1240000000000001</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C38" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B39" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="19">
+        <v>4.0940000000000003</v>
+      </c>
+      <c r="D39" s="19">
+        <v>3.9350000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B40" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="19">
+        <v>3.677</v>
+      </c>
+      <c r="D40" s="19">
+        <v>3.3610000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B41" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" s="19">
+        <v>3.7829999999999999</v>
+      </c>
+      <c r="D41" s="19">
+        <v>3.645</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B42" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="19">
-        <v>3.1280000000000001</v>
-      </c>
-      <c r="C4" s="19">
-        <v>3.2469999999999999</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="19" t="s">
+      <c r="C42" s="19">
+        <v>3.6709999999999998</v>
+      </c>
+      <c r="D42" s="19">
+        <v>3.4119999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B43" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="19">
-        <v>2.9660000000000002</v>
-      </c>
-      <c r="C5" s="19">
-        <v>2.8540000000000001</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="19" t="s">
+      <c r="C43" s="19">
+        <v>3.254</v>
+      </c>
+      <c r="D43" s="19">
+        <v>3.0619999999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B44" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="19">
-        <v>2.6859999999999999</v>
-      </c>
-      <c r="C6" s="19">
-        <v>2.7530000000000001</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="19" t="s">
+      <c r="C44" s="19">
+        <v>3.6230000000000002</v>
+      </c>
+      <c r="D44" s="19">
+        <v>2.9969999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B45" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="19">
-        <v>2.57</v>
-      </c>
-      <c r="C7" s="19">
-        <v>2.6070000000000002</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" s="19" t="s">
+      <c r="C45" s="19">
+        <v>2.629</v>
+      </c>
+      <c r="D45" s="19">
+        <v>3.71</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B46" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="19">
-        <v>2.1509999999999998</v>
-      </c>
-      <c r="C8" s="19">
-        <v>3.4039999999999999</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="19" t="s">
+      <c r="C46" s="19">
+        <v>2.7429999999999999</v>
+      </c>
+      <c r="D46" s="19">
+        <v>3.0649999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B47" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="19">
-        <v>2.093</v>
-      </c>
-      <c r="C9" s="19">
-        <v>2.5390000000000001</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" s="19" t="s">
+      <c r="C47" s="19">
+        <v>2.9540000000000002</v>
+      </c>
+      <c r="D47" s="19">
+        <v>3.2130000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B48" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="19">
-        <v>2.2330000000000001</v>
-      </c>
-      <c r="C10" s="19">
-        <v>2.7730000000000001</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="19">
-        <v>2.419</v>
-      </c>
-      <c r="C11" s="19">
-        <v>3.1240000000000001</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B38" s="19" t="s">
+      <c r="C48" s="19">
+        <v>2.9089999999999998</v>
+      </c>
+      <c r="D48" s="19">
+        <v>3.3010000000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C51" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D51" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B52" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A39" s="19" t="s">
+      <c r="C52" s="19">
+        <v>4.3440000000000003</v>
+      </c>
+      <c r="D52" s="19">
+        <v>4.1120000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B53" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B39" s="19">
-        <v>4.0940000000000003</v>
-      </c>
-      <c r="C39" s="19">
-        <v>3.9350000000000001</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A40" s="19" t="s">
+      <c r="C53" s="19">
+        <v>3.7719999999999998</v>
+      </c>
+      <c r="D53" s="19">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B54" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B40" s="19">
-        <v>3.677</v>
-      </c>
-      <c r="C40" s="19">
-        <v>3.3610000000000002</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A41" s="19" t="s">
+      <c r="C54" s="19">
+        <v>4.0709999999999997</v>
+      </c>
+      <c r="D54" s="19">
+        <v>3.9449999999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B55" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="19">
-        <v>3.7829999999999999</v>
-      </c>
-      <c r="C41" s="19">
-        <v>3.645</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A42" s="19" t="s">
+      <c r="C55" s="19">
+        <v>3.5880000000000001</v>
+      </c>
+      <c r="D55" s="19">
+        <v>3.4369999999999998</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B56" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B42" s="19">
-        <v>3.6709999999999998</v>
-      </c>
-      <c r="C42" s="19">
+      <c r="C56" s="19">
+        <v>3.1309999999999998</v>
+      </c>
+      <c r="D56" s="19">
+        <v>3.1640000000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B57" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57" s="19">
+        <v>3.444</v>
+      </c>
+      <c r="D57" s="19">
+        <v>2.9820000000000002</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B58" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" s="19">
+        <v>2.758</v>
+      </c>
+      <c r="D58" s="19">
+        <v>3.754</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B59" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59" s="19">
+        <v>2.956</v>
+      </c>
+      <c r="D59" s="19">
         <v>3.4119999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A43" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="B43" s="19">
-        <v>3.254</v>
-      </c>
-      <c r="C43" s="19">
-        <v>3.0619999999999998</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A44" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="B44" s="19">
-        <v>3.6230000000000002</v>
-      </c>
-      <c r="C44" s="19">
-        <v>2.9969999999999999</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A45" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B45" s="19">
-        <v>2.629</v>
-      </c>
-      <c r="C45" s="19">
-        <v>3.71</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A46" s="19" t="s">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B60" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B46" s="19">
-        <v>2.7429999999999999</v>
-      </c>
-      <c r="C46" s="19">
-        <v>3.0649999999999999</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A47" s="19" t="s">
+      <c r="C60" s="19">
+        <v>3.1150000000000002</v>
+      </c>
+      <c r="D60" s="19">
+        <v>3.5390000000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B61" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B47" s="19">
-        <v>2.9540000000000002</v>
-      </c>
-      <c r="C47" s="19">
-        <v>3.2130000000000001</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A48" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="B48" s="19">
-        <v>2.9089999999999998</v>
-      </c>
-      <c r="C48" s="19">
-        <v>3.3010000000000002</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B51" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C51" s="19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A52" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B52" s="19">
-        <v>4.3440000000000003</v>
-      </c>
-      <c r="C52" s="19">
-        <v>4.1120000000000001</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A53" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B53" s="19">
-        <v>3.7719999999999998</v>
-      </c>
-      <c r="C53" s="19">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A54" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B54" s="19">
-        <v>4.0709999999999997</v>
-      </c>
-      <c r="C54" s="19">
-        <v>3.9449999999999998</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A55" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="B55" s="19">
-        <v>3.5880000000000001</v>
-      </c>
-      <c r="C55" s="19">
-        <v>3.4369999999999998</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A56" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="B56" s="19">
-        <v>3.1309999999999998</v>
-      </c>
-      <c r="C56" s="19">
-        <v>3.1640000000000001</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A57" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="B57" s="19">
-        <v>3.444</v>
-      </c>
-      <c r="C57" s="19">
-        <v>2.9820000000000002</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A58" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B58" s="19">
-        <v>2.758</v>
-      </c>
-      <c r="C58" s="19">
-        <v>3.754</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A59" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="B59" s="19">
-        <v>2.956</v>
-      </c>
-      <c r="C59" s="19">
-        <v>3.4119999999999999</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A60" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="B60" s="19">
-        <v>3.1150000000000002</v>
-      </c>
-      <c r="C60" s="19">
-        <v>3.5390000000000001</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A61" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="B61" s="19">
+      <c r="C61" s="19">
         <v>3.0310000000000001</v>
       </c>
-      <c r="C61" s="19">
+      <c r="D61" s="19">
         <v>3.6589999999999998</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A2:A8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E2F1B4-7BC8-4065-82D4-E2F1E0723FAD}">
-  <dimension ref="A1:O10"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE18947-7650-40E0-B1AF-F51836C4BD69}">
+  <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection sqref="A1:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="14.5625" style="51" customWidth="1"/>
+    <col min="2" max="2" width="29.875" style="51" customWidth="1"/>
+    <col min="3" max="20" width="9" style="50"/>
+    <col min="21" max="16384" width="9" style="51"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A1" s="114" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="116" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="97" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="101"/>
+      <c r="K1" s="101"/>
+      <c r="L1" s="101"/>
+      <c r="M1" s="101"/>
+      <c r="N1" s="102"/>
+      <c r="O1" s="105" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="106"/>
+      <c r="Q1" s="106"/>
+      <c r="R1" s="106"/>
+      <c r="S1" s="106"/>
+      <c r="T1" s="107"/>
+    </row>
+    <row r="2" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="114"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="125"/>
+      <c r="E2" s="94" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="125"/>
+      <c r="G2" s="94" t="s">
+        <v>107</v>
+      </c>
+      <c r="H2" s="96"/>
+      <c r="I2" s="103" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" s="137"/>
+      <c r="K2" s="103" t="s">
+        <v>106</v>
+      </c>
+      <c r="L2" s="103"/>
+      <c r="M2" s="138" t="s">
+        <v>107</v>
+      </c>
+      <c r="N2" s="104"/>
+      <c r="O2" s="108" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" s="139"/>
+      <c r="Q2" s="108" t="s">
+        <v>106</v>
+      </c>
+      <c r="R2" s="139"/>
+      <c r="S2" s="108" t="s">
+        <v>107</v>
+      </c>
+      <c r="T2" s="109"/>
+    </row>
+    <row r="3" spans="1:20" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="115"/>
+      <c r="B3" s="117"/>
+      <c r="C3" s="126" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="127" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" s="128" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" s="129" t="s">
+        <v>104</v>
+      </c>
+      <c r="G3" s="127" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" s="130" t="s">
+        <v>104</v>
+      </c>
+      <c r="I3" s="131" t="s">
+        <v>103</v>
+      </c>
+      <c r="J3" s="135" t="s">
+        <v>104</v>
+      </c>
+      <c r="K3" s="133" t="s">
+        <v>103</v>
+      </c>
+      <c r="L3" s="135" t="s">
+        <v>104</v>
+      </c>
+      <c r="M3" s="133" t="s">
+        <v>103</v>
+      </c>
+      <c r="N3" s="132" t="s">
+        <v>104</v>
+      </c>
+      <c r="O3" s="140" t="s">
+        <v>103</v>
+      </c>
+      <c r="P3" s="141" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q3" s="142" t="s">
+        <v>103</v>
+      </c>
+      <c r="R3" s="146" t="s">
+        <v>104</v>
+      </c>
+      <c r="S3" s="142" t="s">
+        <v>103</v>
+      </c>
+      <c r="T3" s="143" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="43.15" thickTop="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="118" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="91" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="84">
+        <v>0.4</v>
+      </c>
+      <c r="D4" s="93">
+        <v>0.66</v>
+      </c>
+      <c r="E4" s="122">
+        <v>0.36</v>
+      </c>
+      <c r="F4" s="121">
+        <v>0.74</v>
+      </c>
+      <c r="G4" s="84">
+        <v>0.4</v>
+      </c>
+      <c r="H4" s="88">
+        <v>0.66</v>
+      </c>
+      <c r="I4" s="144">
+        <v>0.39</v>
+      </c>
+      <c r="J4" s="136">
+        <v>0.78</v>
+      </c>
+      <c r="K4" s="145">
+        <v>0.48</v>
+      </c>
+      <c r="L4" s="136">
+        <v>0.68</v>
+      </c>
+      <c r="M4" s="84">
+        <v>0.41</v>
+      </c>
+      <c r="N4" s="111">
+        <v>0.74</v>
+      </c>
+      <c r="O4" s="84">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="P4" s="136">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="Q4" s="134">
+        <v>0.68</v>
+      </c>
+      <c r="R4" s="147">
+        <v>0.5</v>
+      </c>
+      <c r="S4" s="84"/>
+      <c r="T4" s="111"/>
+    </row>
+    <row r="5" spans="1:20" ht="57" x14ac:dyDescent="0.5">
+      <c r="A5" s="119" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="91" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="84">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="121">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E5" s="84">
+        <v>0.3</v>
+      </c>
+      <c r="F5" s="121">
+        <v>0.68</v>
+      </c>
+      <c r="G5" s="84">
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="88">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I5" s="144">
+        <v>0.48</v>
+      </c>
+      <c r="J5" s="136">
+        <v>0.73</v>
+      </c>
+      <c r="K5" s="84">
+        <v>0.27</v>
+      </c>
+      <c r="L5" s="136">
+        <v>0.73</v>
+      </c>
+      <c r="M5" s="84">
+        <v>0.35</v>
+      </c>
+      <c r="N5" s="111">
+        <v>0.75</v>
+      </c>
+      <c r="O5" s="84">
+        <v>0.21</v>
+      </c>
+      <c r="P5" s="136">
+        <v>0.85</v>
+      </c>
+      <c r="Q5" s="145">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="R5" s="136">
+        <v>0.82</v>
+      </c>
+      <c r="S5" s="84"/>
+      <c r="T5" s="111"/>
+    </row>
+    <row r="6" spans="1:20" ht="28.5" x14ac:dyDescent="0.5">
+      <c r="A6" s="119" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="91" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="84">
+        <v>0.25</v>
+      </c>
+      <c r="D6" s="121">
+        <v>0.84</v>
+      </c>
+      <c r="E6" s="84">
+        <v>0.3</v>
+      </c>
+      <c r="F6" s="121">
+        <v>0.84</v>
+      </c>
+      <c r="G6" s="84">
+        <v>0.25</v>
+      </c>
+      <c r="H6" s="88">
+        <v>0.84</v>
+      </c>
+      <c r="I6" s="144">
+        <v>0.47</v>
+      </c>
+      <c r="J6" s="136">
+        <v>0.77</v>
+      </c>
+      <c r="K6" s="84">
+        <v>0.49</v>
+      </c>
+      <c r="L6" s="136">
+        <v>0.66</v>
+      </c>
+      <c r="M6" s="84">
+        <v>0.46</v>
+      </c>
+      <c r="N6" s="111">
+        <v>0.73</v>
+      </c>
+      <c r="O6" s="110">
+        <v>0.61</v>
+      </c>
+      <c r="P6" s="136">
+        <v>0.61</v>
+      </c>
+      <c r="Q6" s="134">
+        <v>0.71</v>
+      </c>
+      <c r="R6" s="123">
+        <v>0.53</v>
+      </c>
+      <c r="T6" s="111"/>
+    </row>
+    <row r="7" spans="1:20" ht="42.75" x14ac:dyDescent="0.5">
+      <c r="A7" s="119" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="91" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="84">
+        <v>0.33</v>
+      </c>
+      <c r="D7" s="93">
+        <v>0.8</v>
+      </c>
+      <c r="E7" s="122">
+        <v>0.32</v>
+      </c>
+      <c r="F7" s="121">
+        <v>0.81</v>
+      </c>
+      <c r="G7" s="84">
+        <v>0.33</v>
+      </c>
+      <c r="H7" s="88">
+        <v>0.8</v>
+      </c>
+      <c r="I7" s="144">
+        <v>0.33</v>
+      </c>
+      <c r="J7" s="136">
+        <v>0.8</v>
+      </c>
+      <c r="K7" s="84">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L7" s="136">
+        <v>0.84</v>
+      </c>
+      <c r="M7" s="84">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="N7" s="111">
+        <v>0.83</v>
+      </c>
+      <c r="O7" s="84">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="P7" s="136">
+        <v>0.87</v>
+      </c>
+      <c r="Q7" s="145">
+        <v>0.33</v>
+      </c>
+      <c r="R7" s="136">
+        <v>0.83</v>
+      </c>
+      <c r="S7" s="84"/>
+      <c r="T7" s="111"/>
+    </row>
+    <row r="8" spans="1:20" ht="42.75" x14ac:dyDescent="0.5">
+      <c r="A8" s="119" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="91" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="84">
+        <v>0.4</v>
+      </c>
+      <c r="D8" s="121">
+        <v>0.52</v>
+      </c>
+      <c r="E8" s="84">
+        <v>0.32</v>
+      </c>
+      <c r="F8" s="121">
+        <v>0.6</v>
+      </c>
+      <c r="G8" s="84">
+        <v>0.4</v>
+      </c>
+      <c r="H8" s="88">
+        <v>0.52</v>
+      </c>
+      <c r="I8" s="144">
+        <v>0.41</v>
+      </c>
+      <c r="J8" s="136">
+        <v>0.53</v>
+      </c>
+      <c r="K8" s="84">
+        <v>0.2</v>
+      </c>
+      <c r="L8" s="136">
+        <v>0.62</v>
+      </c>
+      <c r="M8" s="84">
+        <v>0.34</v>
+      </c>
+      <c r="N8" s="111">
+        <v>0.48</v>
+      </c>
+      <c r="O8" s="84">
+        <v>0.32</v>
+      </c>
+      <c r="P8" s="136">
+        <v>0.61</v>
+      </c>
+      <c r="Q8" s="145">
+        <v>0.24</v>
+      </c>
+      <c r="R8" s="136">
+        <v>0.69</v>
+      </c>
+      <c r="S8" s="84"/>
+      <c r="T8" s="111"/>
+    </row>
+    <row r="9" spans="1:20" ht="42.75" x14ac:dyDescent="0.5">
+      <c r="A9" s="119" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="91" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="50">
+        <v>0.6</v>
+      </c>
+      <c r="D9" s="123">
+        <v>0.43</v>
+      </c>
+      <c r="E9" s="84">
+        <v>0.54</v>
+      </c>
+      <c r="F9" s="121">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G9" s="50">
+        <v>0.6</v>
+      </c>
+      <c r="H9" s="89">
+        <v>0.43</v>
+      </c>
+      <c r="I9" s="144">
+        <v>0.5</v>
+      </c>
+      <c r="J9" s="136">
+        <v>0.72</v>
+      </c>
+      <c r="K9" s="84">
+        <v>0.34</v>
+      </c>
+      <c r="L9" s="136">
+        <v>0.73</v>
+      </c>
+      <c r="M9" s="84">
+        <v>0.41</v>
+      </c>
+      <c r="N9" s="111">
+        <v>0.74</v>
+      </c>
+      <c r="O9" s="84">
+        <v>0.36</v>
+      </c>
+      <c r="P9" s="136">
+        <v>0.79</v>
+      </c>
+      <c r="Q9" s="145">
+        <v>0.4</v>
+      </c>
+      <c r="R9" s="136">
+        <v>0.77</v>
+      </c>
+      <c r="S9" s="84"/>
+      <c r="T9" s="111"/>
+    </row>
+    <row r="10" spans="1:20" ht="42.75" x14ac:dyDescent="0.5">
+      <c r="A10" s="119" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="91" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="50">
+        <v>0.61</v>
+      </c>
+      <c r="D10" s="123">
+        <v>0.21</v>
+      </c>
+      <c r="E10" s="84">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F10" s="121">
+        <v>0.49</v>
+      </c>
+      <c r="G10" s="50">
+        <v>0.61</v>
+      </c>
+      <c r="H10" s="89">
+        <v>0.21</v>
+      </c>
+      <c r="I10" s="144">
+        <v>0.41</v>
+      </c>
+      <c r="J10" s="136">
+        <v>0.7</v>
+      </c>
+      <c r="K10" s="84">
+        <v>0.21</v>
+      </c>
+      <c r="L10" s="136">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="M10" s="84">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="N10" s="111">
+        <v>0.66</v>
+      </c>
+      <c r="O10" s="84">
+        <v>0.26</v>
+      </c>
+      <c r="P10" s="136">
+        <v>0.77</v>
+      </c>
+      <c r="Q10" s="145">
+        <v>0.25</v>
+      </c>
+      <c r="R10" s="136">
+        <v>0.67</v>
+      </c>
+      <c r="S10" s="84"/>
+      <c r="T10" s="111"/>
+    </row>
+    <row r="11" spans="1:20" ht="28.5" x14ac:dyDescent="0.5">
+      <c r="A11" s="119" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="91" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="50">
+        <v>0.75</v>
+      </c>
+      <c r="D11" s="123">
+        <v>0.33</v>
+      </c>
+      <c r="E11" s="50">
+        <v>0.76</v>
+      </c>
+      <c r="F11" s="123">
+        <v>0.33</v>
+      </c>
+      <c r="G11" s="50">
+        <v>0.75</v>
+      </c>
+      <c r="H11" s="89">
+        <v>0.33</v>
+      </c>
+      <c r="I11" s="110">
+        <v>0.85</v>
+      </c>
+      <c r="J11" s="123">
+        <v>0.39</v>
+      </c>
+      <c r="K11" s="110">
+        <v>0.82</v>
+      </c>
+      <c r="L11" s="123">
+        <v>0.37</v>
+      </c>
+      <c r="M11" s="110">
+        <v>0.84</v>
+      </c>
+      <c r="N11" s="89">
+        <v>0.38</v>
+      </c>
+      <c r="O11" s="110">
+        <v>0.84</v>
+      </c>
+      <c r="P11" s="123">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="Q11" s="134">
+        <v>0.83</v>
+      </c>
+      <c r="R11" s="123">
+        <v>0.35</v>
+      </c>
+      <c r="T11" s="89"/>
+    </row>
+    <row r="12" spans="1:20" ht="42.75" x14ac:dyDescent="0.5">
+      <c r="A12" s="119" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="91" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="50">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D12" s="123">
+        <v>0.39</v>
+      </c>
+      <c r="E12" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="F12" s="123">
+        <v>0.22</v>
+      </c>
+      <c r="G12" s="50">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="H12" s="89">
+        <v>0.39</v>
+      </c>
+      <c r="I12" s="110">
+        <v>0.71</v>
+      </c>
+      <c r="J12" s="123">
+        <v>0.38</v>
+      </c>
+      <c r="K12" s="110">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L12" s="123">
+        <v>0.15</v>
+      </c>
+      <c r="M12" s="110">
+        <v>0.63</v>
+      </c>
+      <c r="N12" s="89">
+        <v>0.3</v>
+      </c>
+      <c r="O12" s="110">
+        <v>0.77</v>
+      </c>
+      <c r="P12" s="123">
+        <v>0.23</v>
+      </c>
+      <c r="Q12" s="134">
+        <v>0.69</v>
+      </c>
+      <c r="R12" s="123">
+        <v>0.18</v>
+      </c>
+      <c r="T12" s="89"/>
+    </row>
+    <row r="13" spans="1:20" ht="31.9" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="120" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="86" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="92">
+        <v>0.78</v>
+      </c>
+      <c r="D13" s="124">
+        <v>0.32</v>
+      </c>
+      <c r="E13" s="87">
+        <v>0.76</v>
+      </c>
+      <c r="F13" s="124">
+        <v>0.3</v>
+      </c>
+      <c r="G13" s="87">
+        <v>0.78</v>
+      </c>
+      <c r="H13" s="90">
+        <v>0.32</v>
+      </c>
+      <c r="I13" s="112">
+        <v>0.72</v>
+      </c>
+      <c r="J13" s="124">
+        <v>0.42</v>
+      </c>
+      <c r="K13" s="113">
+        <v>0.77</v>
+      </c>
+      <c r="L13" s="124">
+        <v>0.39</v>
+      </c>
+      <c r="M13" s="113">
+        <v>0.75</v>
+      </c>
+      <c r="N13" s="90">
+        <v>0.4</v>
+      </c>
+      <c r="O13" s="112">
+        <v>0.82</v>
+      </c>
+      <c r="P13" s="124">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="Q13" s="113">
+        <v>0.83</v>
+      </c>
+      <c r="R13" s="124">
+        <v>0.3</v>
+      </c>
+      <c r="S13" s="113"/>
+      <c r="T13" s="90"/>
+    </row>
+    <row r="14" spans="1:20" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5"/>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="C16" s="85"/>
+      <c r="I16" s="85"/>
+      <c r="O16" s="85"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="O1:T1"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="B1:B3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E2F1B4-7BC8-4065-82D4-E2F1E0723FAD}">
+  <dimension ref="A1:P8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -6123,378 +7921,334 @@
     <col min="3" max="3" width="13.625" customWidth="1"/>
     <col min="7" max="7" width="14.6875" customWidth="1"/>
     <col min="8" max="8" width="16.0625" customWidth="1"/>
+    <col min="11" max="11" width="13.0625" customWidth="1"/>
     <col min="12" max="12" width="14.375" customWidth="1"/>
-    <col min="13" max="13" width="12.9375" customWidth="1"/>
+    <col min="13" max="13" width="13.5" customWidth="1"/>
+    <col min="14" max="14" width="12.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A1" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="G1" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A2" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="23">
+        <v>2.83</v>
+      </c>
+      <c r="C2" s="23">
+        <v>3.04</v>
+      </c>
+      <c r="D2" s="23">
+        <v>-1.1059000000000001</v>
+      </c>
+      <c r="E2" s="24">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="23">
+        <v>3.11</v>
+      </c>
+      <c r="H2" s="23">
+        <v>3.16</v>
+      </c>
+      <c r="I2" s="23">
+        <v>-0.35799999999999998</v>
+      </c>
+      <c r="J2" s="24">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="K2" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" s="23">
+        <v>2.74</v>
+      </c>
+      <c r="M2" s="23">
+        <v>3.07</v>
+      </c>
+      <c r="N2" s="23">
+        <v>-7.72</v>
+      </c>
+      <c r="O2" s="24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A3" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="23">
+        <v>2.98</v>
+      </c>
+      <c r="C3" s="23">
+        <v>3.47</v>
+      </c>
+      <c r="D3" s="23">
+        <v>-3.9950000000000001</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="23">
+        <v>2.4</v>
+      </c>
+      <c r="H3" s="23">
+        <v>3.11</v>
+      </c>
+      <c r="I3" s="23">
+        <v>-5.3882000000000003</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="L3" s="23">
+        <v>2.86</v>
+      </c>
+      <c r="M3" s="23">
+        <v>3.7</v>
+      </c>
+      <c r="N3" s="23">
+        <v>-14.87</v>
+      </c>
+      <c r="O3" s="24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="K4" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="L4" s="9">
+        <v>2.88</v>
+      </c>
+      <c r="M4" s="9">
+        <v>3.49</v>
+      </c>
+      <c r="N4" s="36">
+        <v>-12.68</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="K5" s="34"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A6" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="41" t="s">
+      <c r="B6" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E6" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="I1" s="44" t="s">
+      <c r="F6" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="44" t="s">
+      <c r="J6" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="M1" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="N1" s="46" t="s">
+      <c r="K6" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="M6" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="N6" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="O6" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="46" t="s">
+      <c r="P6" s="26" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A2" s="42"/>
-      <c r="B2" s="40" t="s">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A7" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="40" t="s">
+      <c r="B7" s="23">
+        <v>2.82</v>
+      </c>
+      <c r="C7" s="23">
+        <v>2.98</v>
+      </c>
+      <c r="D7" s="23">
+        <v>-0.56100000000000005</v>
+      </c>
+      <c r="E7" s="24">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="F7" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="40" t="s">
+      <c r="G7" s="23">
+        <v>3.11</v>
+      </c>
+      <c r="H7" s="23">
+        <v>2.4</v>
+      </c>
+      <c r="I7" s="23">
+        <v>2.81</v>
+      </c>
+      <c r="J7" s="24">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="K7" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A3" s="42"/>
-      <c r="B3" s="33">
-        <v>2.83</v>
-      </c>
-      <c r="C3" s="33">
+      <c r="L7" s="23">
+        <v>2.74</v>
+      </c>
+      <c r="M7" s="23">
+        <v>2.86</v>
+      </c>
+      <c r="N7" s="24">
+        <v>2.88</v>
+      </c>
+      <c r="O7" s="23">
+        <v>2.81</v>
+      </c>
+      <c r="P7" s="24">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A8" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="23">
         <v>3.04</v>
       </c>
-      <c r="D3" s="33">
-        <v>-1.1059000000000001</v>
-      </c>
-      <c r="E3" s="38">
-        <v>0.27700000000000002</v>
-      </c>
-      <c r="F3" s="43"/>
-      <c r="G3" s="33">
+      <c r="C8" s="23">
+        <v>3.48</v>
+      </c>
+      <c r="D8" s="23">
+        <v>-1.6065</v>
+      </c>
+      <c r="E8" s="24">
+        <v>0.1129</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" s="23">
+        <v>3.16</v>
+      </c>
+      <c r="H8" s="23">
         <v>3.11</v>
       </c>
-      <c r="H3" s="33">
-        <v>3.16</v>
-      </c>
-      <c r="I3" s="33">
-        <v>-0.35799999999999998</v>
-      </c>
-      <c r="J3" s="38">
-        <v>0.72099999999999997</v>
-      </c>
-      <c r="K3" s="45"/>
-      <c r="L3" s="33">
+      <c r="I8" s="23">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="J8" s="24">
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="K8" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="L8" s="23">
+        <v>3.07</v>
+      </c>
+      <c r="M8" s="23">
         <v>3.11</v>
       </c>
-      <c r="M3" s="33">
-        <v>3.16</v>
-      </c>
-      <c r="N3" s="33">
-        <v>-0.35799999999999998</v>
-      </c>
-      <c r="O3" s="38">
-        <v>0.72099999999999997</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A4" s="42"/>
-      <c r="B4" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A5" s="42"/>
-      <c r="B5" s="33">
-        <v>2.98</v>
-      </c>
-      <c r="C5" s="33">
-        <v>3.47</v>
-      </c>
-      <c r="D5" s="33">
-        <v>-3.9950000000000001</v>
-      </c>
-      <c r="E5" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="43"/>
-      <c r="G5" s="33">
-        <v>2.4</v>
-      </c>
-      <c r="H5" s="33">
-        <v>3.11</v>
-      </c>
-      <c r="I5" s="33">
-        <v>-5.3882000000000003</v>
-      </c>
-      <c r="J5" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="45"/>
-      <c r="L5" s="33">
-        <v>2.4</v>
-      </c>
-      <c r="M5" s="33">
-        <v>3.11</v>
-      </c>
-      <c r="N5" s="33">
-        <v>-5.3882000000000003</v>
-      </c>
-      <c r="O5" s="38" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A8" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="H8" s="44" t="s">
-        <v>80</v>
-      </c>
-      <c r="I8" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="L8" s="46" t="s">
-        <v>79</v>
-      </c>
-      <c r="M8" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="N8" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="O8" s="46" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A9" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="33">
-        <v>2.82</v>
-      </c>
-      <c r="C9" s="33">
-        <v>2.98</v>
-      </c>
-      <c r="D9" s="33">
-        <v>-0.56100000000000005</v>
-      </c>
-      <c r="E9" s="38">
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="F9" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="G9" s="33">
-        <v>3.11</v>
-      </c>
-      <c r="H9" s="33">
-        <v>2.4</v>
-      </c>
-      <c r="I9" s="33">
-        <v>2.81</v>
-      </c>
-      <c r="J9" s="38">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="K9" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="L9" s="33">
-        <v>3.11</v>
-      </c>
-      <c r="M9" s="33">
-        <v>2.4</v>
-      </c>
-      <c r="N9" s="33">
-        <v>2.81</v>
-      </c>
-      <c r="O9" s="38">
-        <v>6.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A10" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" s="33">
-        <v>3.04</v>
-      </c>
-      <c r="C10" s="33">
-        <v>3.48</v>
-      </c>
-      <c r="D10" s="33">
-        <v>-1.6065</v>
-      </c>
-      <c r="E10" s="38">
-        <v>0.1129</v>
-      </c>
-      <c r="F10" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="G10" s="33">
-        <v>3.16</v>
-      </c>
-      <c r="H10" s="33">
-        <v>3.11</v>
-      </c>
-      <c r="I10" s="33">
+      <c r="N8" s="24">
+        <v>3.49</v>
+      </c>
+      <c r="O8" s="23">
         <v>0.20699999999999999</v>
       </c>
-      <c r="J10" s="38">
+      <c r="P8" s="24">
         <v>0.83599999999999997</v>
       </c>
-      <c r="K10" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="L10" s="33">
-        <v>3.16</v>
-      </c>
-      <c r="M10" s="33">
-        <v>3.11</v>
-      </c>
-      <c r="N10" s="33">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="O10" s="38">
-        <v>0.83599999999999997</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="K1:K5"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="A1:A5"/>
-    <mergeCell ref="F1:F5"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="G4:J4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB1568F0-3754-4110-ADDE-1A6EDD471F19}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A4FC0C-94F6-4EE7-A7D0-F02B7768E222}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>